<commit_message>
Implement all stocks part
</commit_message>
<xml_diff>
--- a/Files/Total/xlsx Files/order_history.xlsx
+++ b/Files/Total/xlsx Files/order_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -34,10 +34,7 @@
     <t>Total</t>
   </si>
   <si>
-    <t>2023-07-15</t>
-  </si>
-  <si>
-    <t>2023-07-19</t>
+    <t>2023-07-18</t>
   </si>
   <si>
     <t>Buy</t>
@@ -46,10 +43,13 @@
     <t>Sell</t>
   </si>
   <si>
-    <t>OKIDOKI</t>
-  </si>
-  <si>
-    <t>EREGL</t>
+    <t>ODAS.IS</t>
+  </si>
+  <si>
+    <t>EREGL.IS</t>
+  </si>
+  <si>
+    <t>SISE.IS</t>
   </si>
 </sst>
 </file>
@@ -407,7 +407,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -438,19 +438,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>1000</v>
+        <v>34</v>
       </c>
       <c r="F2">
-        <v>23000</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -458,19 +458,19 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E3">
-        <v>-500</v>
+        <v>34</v>
       </c>
       <c r="F3">
-        <v>-5000</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -481,56 +481,16 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="E4">
-        <v>1000</v>
+        <v>-3</v>
       </c>
       <c r="F4">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>10</v>
-      </c>
-      <c r="F5">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6">
-        <v>23</v>
-      </c>
-      <c r="E6">
-        <v>1000</v>
-      </c>
-      <c r="F6">
-        <v>23000</v>
+        <v>-102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>